<commit_message>
Complete Test spreadsheet (remediation not complete)
</commit_message>
<xml_diff>
--- a/docs/Tests.xlsx
+++ b/docs/Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Data Validation" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>Table</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Data Source</t>
   </si>
   <si>
-    <t>Constraints</t>
-  </si>
-  <si>
     <t>TestID</t>
   </si>
   <si>
@@ -65,15 +62,9 @@
     <t>id</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>preferences</t>
   </si>
   <si>
-    <t>[PreferenceSchema]</t>
-  </si>
-  <si>
     <t>when?</t>
   </si>
   <si>
@@ -83,21 +74,12 @@
     <t>To get spotify recommendations</t>
   </si>
   <si>
-    <t>after getting recommendations</t>
-  </si>
-  <si>
     <t>[SongSchema]</t>
   </si>
   <si>
     <t>while listening to song</t>
   </si>
   <si>
-    <t>after song finishes</t>
-  </si>
-  <si>
-    <t>uri</t>
-  </si>
-  <si>
     <t>Page Name</t>
   </si>
   <si>
@@ -176,21 +158,6 @@
     <t>UI06</t>
   </si>
   <si>
-    <t>queue</t>
-  </si>
-  <si>
-    <t>playlist</t>
-  </si>
-  <si>
-    <t>playlist-&gt;queue</t>
-  </si>
-  <si>
-    <t>after song finishes, if song is enjoyed</t>
-  </si>
-  <si>
-    <t>songs</t>
-  </si>
-  <si>
     <t>Spotify</t>
   </si>
   <si>
@@ -209,21 +176,6 @@
     <t>DB05</t>
   </si>
   <si>
-    <t>DB06</t>
-  </si>
-  <si>
-    <t>DB07</t>
-  </si>
-  <si>
-    <t>written by DB04 (Spotify)</t>
-  </si>
-  <si>
-    <t>written by DB05 (Spotify)</t>
-  </si>
-  <si>
-    <t>array length?</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -242,7 +194,40 @@
     <t>UIB02</t>
   </si>
   <si>
+    <t>UI07</t>
+  </si>
+  <si>
     <t>See the Source button on homepage unresponsive</t>
+  </si>
+  <si>
+    <t>Play</t>
+  </si>
+  <si>
+    <t>UI08</t>
+  </si>
+  <si>
+    <t>UI09</t>
+  </si>
+  <si>
+    <t>UI10</t>
+  </si>
+  <si>
+    <t>UIB03</t>
+  </si>
+  <si>
+    <t>About button on play page does not redirect to homepage before trying to access #content</t>
+  </si>
+  <si>
+    <t>On initial signin</t>
+  </si>
+  <si>
+    <t>written by DB05/DB03 (Spotify)</t>
+  </si>
+  <si>
+    <t>DBB01</t>
+  </si>
+  <si>
+    <t>New preferences are not added to preference list while listening</t>
   </si>
 </sst>
 </file>
@@ -278,8 +263,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,9 +562,9 @@
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -601,181 +587,135 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
         <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -785,136 +725,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -924,17 +932,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.88671875" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
+    <col min="3" max="3" width="75" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
@@ -942,56 +950,99 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43443</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="F3" s="1">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Tests spreadsheet (remediation incomplete)
</commit_message>
<xml_diff>
--- a/docs/Tests.xlsx
+++ b/docs/Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Data Validation" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>Table</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Data Source</t>
   </si>
   <si>
-    <t>Constraints</t>
-  </si>
-  <si>
     <t>TestID</t>
   </si>
   <si>
@@ -65,15 +62,9 @@
     <t>id</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>preferences</t>
   </si>
   <si>
-    <t>[PreferenceSchema]</t>
-  </si>
-  <si>
     <t>when?</t>
   </si>
   <si>
@@ -83,21 +74,12 @@
     <t>To get spotify recommendations</t>
   </si>
   <si>
-    <t>after getting recommendations</t>
-  </si>
-  <si>
     <t>[SongSchema]</t>
   </si>
   <si>
     <t>while listening to song</t>
   </si>
   <si>
-    <t>after song finishes</t>
-  </si>
-  <si>
-    <t>uri</t>
-  </si>
-  <si>
     <t>Page Name</t>
   </si>
   <si>
@@ -176,21 +158,6 @@
     <t>UI06</t>
   </si>
   <si>
-    <t>queue</t>
-  </si>
-  <si>
-    <t>playlist</t>
-  </si>
-  <si>
-    <t>playlist-&gt;queue</t>
-  </si>
-  <si>
-    <t>after song finishes, if song is enjoyed</t>
-  </si>
-  <si>
-    <t>songs</t>
-  </si>
-  <si>
     <t>Spotify</t>
   </si>
   <si>
@@ -209,21 +176,6 @@
     <t>DB05</t>
   </si>
   <si>
-    <t>DB06</t>
-  </si>
-  <si>
-    <t>DB07</t>
-  </si>
-  <si>
-    <t>written by DB04 (Spotify)</t>
-  </si>
-  <si>
-    <t>written by DB05 (Spotify)</t>
-  </si>
-  <si>
-    <t>array length?</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -264,6 +216,18 @@
   </si>
   <si>
     <t>About button on play page does not redirect to homepage before trying to access #content</t>
+  </si>
+  <si>
+    <t>On initial signin</t>
+  </si>
+  <si>
+    <t>written by DB05/DB03 (Spotify)</t>
+  </si>
+  <si>
+    <t>DBB01</t>
+  </si>
+  <si>
+    <t>New preferences are not added to preference list while listening</t>
   </si>
 </sst>
 </file>
@@ -582,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,9 +562,9 @@
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -623,181 +587,135 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
         <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -822,189 +740,189 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1014,10 +932,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,39 +950,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F2" s="1">
         <v>43443</v>
@@ -1072,19 +990,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F3" s="1">
         <v>43443</v>
@@ -1092,22 +1010,39 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F4" s="1">
         <v>43443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>